<commit_message>
replace nfdi4pso terms in community and repository templates
</commit_message>
<xml_diff>
--- a/templates/community/MAdLand/MAdLand_bioanalyzer.xlsx
+++ b/templates/community/MAdLand/MAdLand_bioanalyzer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\MAdLand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB41FBF-3E33-4D00-A6A5-4FCEA8BA890D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D9A318-6859-4518-9A7C-4E27DECECDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{A22C094B-EDE5-4910-A95F-8098389FC57B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A22C094B-EDE5-4910-A95F-8098389FC57B}"/>
   </bookViews>
   <sheets>
     <sheet name="Fragment-or Bioanalyzer measure" sheetId="1" r:id="rId1"/>
@@ -50,75 +50,75 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{73862CB4-7BFE-476A-B506-29D38C9C1CB2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=0fe0093a-fcf8-4c63-b0e3-d5172a2ba8fb</t>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{418AE240-F39E-4F5F-B5B6-DBA0C310F0A6}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{DCA5538F-1E69-45CE-816E-75E13DF6D5B1}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{049065B0-8AD0-44C5-B0A4-C58E7897F9AA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{A42C30FA-52E0-4077-9B88-F2629605AB2F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{01615BD7-556B-4F4E-A3E8-8146CB910619}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{03C772B8-E75B-4CF2-B309-68C4EE303874}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{4A5ABA0F-FC93-4AAA-922F-9B39155363CE}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{8B511D67-6AF0-4BBA-9A8B-A226E9E1E4B9}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Source Name</t>
   </si>
@@ -153,15 +153,6 @@
     <t>Term Accession Number (UO:0000180)</t>
   </si>
   <si>
-    <t>Parameter [Volume]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:1000154)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000154)</t>
-  </si>
-  <si>
     <t>Parameter [mass]</t>
   </si>
   <si>
@@ -183,9 +174,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Unit (#2)</t>
-  </si>
-  <si>
     <t>Unit (#3)</t>
   </si>
   <si>
@@ -301,18 +289,29 @@
   </si>
   <si>
     <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Parameter [volume]</t>
+  </si>
+  <si>
+    <t>Term Source REF (EFO:0001715)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (EFO:0001715)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;nanogram per microliter&quot;"/>
-    <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;nanogram&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,12 +334,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -461,7 +454,6 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -493,12 +485,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.00\ &quot;nanogram&quot;"/>
     </dxf>
@@ -510,18 +512,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.00\ &quot;nanogram&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;nanogram per microliter&quot;"/>
@@ -556,25 +546,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03268FEA-4313-4609-B6AC-353B965A6E91}" name="annotationTableToughSnail54" displayName="annotationTableToughSnail54" ref="A1:T2" totalsRowShown="0">
-  <autoFilter ref="A1:T2" xr:uid="{03268FEA-4313-4609-B6AC-353B965A6E91}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03268FEA-4313-4609-B6AC-353B965A6E91}" name="annotationTableToughSnail54" displayName="annotationTableToughSnail54" ref="A1:S2" totalsRowShown="0">
+  <autoFilter ref="A1:S2" xr:uid="{03268FEA-4313-4609-B6AC-353B965A6E91}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{5FCE231F-21F1-4754-9664-1EE3C1303360}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{39A4362B-19DB-4F6F-A0DE-6D2426ABE855}" name="Parameter [nucleic acid]"/>
     <tableColumn id="4" xr3:uid="{EC8CF098-456E-4790-8071-1D4258259D58}" name="Term Source REF (CHEBI:33696)"/>
     <tableColumn id="5" xr3:uid="{0523A3A3-EF97-4606-88EB-DB73D2C8DE90}" name="Term Accession Number (CHEBI:33696)"/>
-    <tableColumn id="18" xr3:uid="{58E953D1-B313-46EF-A048-7300F9F92757}" name="Parameter [mass per unit volume]" dataDxfId="11"/>
-    <tableColumn id="19" xr3:uid="{99CA07EA-7878-431F-862C-7F087FEBDA34}" name="Unit" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{6FC4E9A8-E8DA-4BF8-B231-6C92C261989E}" name="Term Source REF (UO:0000180)" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{DB1297DC-373A-4D38-AA49-7C27B0F834F9}" name="Term Accession Number (UO:0000180)" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{7367C08D-08C9-49B2-A016-878F5E950D8E}" name="Parameter [Volume]" dataDxfId="7"/>
-    <tableColumn id="23" xr3:uid="{EDC4194D-9E1F-47B9-9D98-3A03EA612529}" name="Unit (#2)" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{EBE42A7E-577D-4F85-B470-0B9B67908BE3}" name="Term Source REF (NFDI4PSO:1000154)" dataDxfId="5"/>
-    <tableColumn id="25" xr3:uid="{B6BBD6FA-0CAD-46C5-A88B-81E46BBF2771}" name="Term Accession Number (NFDI4PSO:1000154)" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{8D38D022-4DB5-433C-A903-BEDF22E2EDB6}" name="Parameter [mass]" dataDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{DD3B7EAB-5E81-464D-BAB0-54EEDD2C1A29}" name="Unit (#3)" dataDxfId="2"/>
-    <tableColumn id="28" xr3:uid="{C535BBA3-E1D1-4BFF-8933-028110309F70}" name="Term Source REF (PATO:0000125)" dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{DDC25ED6-1429-4CC9-A365-164C5A2DD5A9}" name="Term Accession Number (PATO:0000125)" dataDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{58E953D1-B313-46EF-A048-7300F9F92757}" name="Parameter [mass per unit volume]" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{99CA07EA-7878-431F-862C-7F087FEBDA34}" name="Unit" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{6FC4E9A8-E8DA-4BF8-B231-6C92C261989E}" name="Term Source REF (UO:0000180)" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{DB1297DC-373A-4D38-AA49-7C27B0F834F9}" name="Term Accession Number (UO:0000180)" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{4627ABDA-3277-422E-B296-072F66CA6B53}" name="Parameter [volume]" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{2CA176F6-87DE-41A3-AD43-74D1CF381B44}" name="Term Source REF (EFO:0001715)" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{776B65BD-0B70-4BC4-8ED1-BB168955D547}" name="Term Accession Number (EFO:0001715)" dataDxfId="0"/>
+    <tableColumn id="26" xr3:uid="{8D38D022-4DB5-433C-A903-BEDF22E2EDB6}" name="Parameter [mass]" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{DD3B7EAB-5E81-464D-BAB0-54EEDD2C1A29}" name="Unit (#3)" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{C535BBA3-E1D1-4BFF-8933-028110309F70}" name="Term Source REF (PATO:0000125)" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{DDC25ED6-1429-4CC9-A365-164C5A2DD5A9}" name="Term Accession Number (PATO:0000125)" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{5527DD0F-2117-41E4-A7E2-855FB4E2A14C}" name="Parameter [RNA Integrity Number value specification]"/>
     <tableColumn id="16" xr3:uid="{6A8E9D3B-914D-444D-BB9B-F85F49E2B975}" name="Term Source REF (OBI:0002137)"/>
     <tableColumn id="17" xr3:uid="{389B398C-C07C-4948-B41B-B53F2E3B6000}" name="Term Accession Number (OBI:0002137)"/>
@@ -585,9 +574,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -625,7 +614,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -731,7 +720,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -873,7 +862,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -916,7 +905,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="417" row="3">
+  <wetp:taskpane dockstate="right" visibility="0" width="882" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="388" row="4">
@@ -947,36 +936,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0770B4E5-CFCC-446B-8D4E-712D5A7D9179}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="32.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="52" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="15.5703125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="36" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="31.5546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +982,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -1002,55 +991,55 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
       <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1064,203 +1053,203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B663E89-2380-497F-9DB6-E7983D99A3C1}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B5" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="9"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="9"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>